<commit_message>
adjusted northwind, and completed third step of power bi
</commit_message>
<xml_diff>
--- a/NorthwindTablesAndColumns.xlsx
+++ b/NorthwindTablesAndColumns.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\YUU-LearnToCode\DataAnalytics\Week_9\W9_Exercises\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C1DBF32D-165E-43B1-8B20-312A6C932B64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A3F8659-2D91-4821-BB45-755516241F84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="336" yWindow="408" windowWidth="21744" windowHeight="12468" xr2:uid="{901F5D27-877F-4C94-89AE-9A9B6ECE5CB6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{901F5D27-877F-4C94-89AE-9A9B6ECE5CB6}"/>
   </bookViews>
   <sheets>
     <sheet name="Northwind Columns" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="149">
   <si>
     <t>table_name</t>
   </si>
@@ -946,10 +946,10 @@
   <dimension ref="A1:N83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D62" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J94" sqref="J94"/>
+      <selection pane="bottomRight" activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2114,7 +2114,7 @@
         <v>1</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="J34" t="s">
         <v>18</v>
@@ -2137,16 +2137,13 @@
         <v>4</v>
       </c>
       <c r="F35" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G35" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I35" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="J35" t="s">
         <v>18</v>
@@ -2169,7 +2166,7 @@
         <v>4</v>
       </c>
       <c r="F36" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G36" t="b">
         <v>1</v>

</xml_diff>